<commit_message>
Fuzzy inference system and matrix representation
</commit_message>
<xml_diff>
--- a/results/eval/eval.xlsx
+++ b/results/eval/eval.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aokim\Documents\Bachelorarbeit\opencv\results\eval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marina/introcs/Bachelorarbeit/opencv/results/eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EA33A5-3948-439F-98DE-AFFDF7015504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EDFF5E-B740-F642-A992-3C18A93C9B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15590" yWindow="1300" windowWidth="14400" windowHeight="7360" xr2:uid="{715AE36E-C2AF-453D-BF97-D90B9BF6E64C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{715AE36E-C2AF-453D-BF97-D90B9BF6E64C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
   <si>
     <t>Event</t>
   </si>
@@ -133,6 +142,21 @@
   </si>
   <si>
     <t>0;l</t>
+  </si>
+  <si>
+    <t>TRAIN</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>SMALL</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -626,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -668,6 +692,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -680,35 +719,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,38 +1048,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783BF86-7641-4C3E-A52C-C236B26E7C81}">
-  <dimension ref="A1:G56"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="119" zoomScaleNormal="17" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1081,8 +1107,11 @@
       <c r="E3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1098,8 +1127,11 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1115,8 +1147,11 @@
       <c r="E5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1132,8 +1167,11 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1149,8 +1187,17 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+    </row>
+    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1166,8 +1213,14 @@
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1183,8 +1236,14 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1200,8 +1259,14 @@
       <c r="E10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1217,8 +1282,14 @@
       <c r="E11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1234,8 +1305,14 @@
       <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,8 +1328,14 @@
       <c r="E13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1268,8 +1351,14 @@
       <c r="E14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1285,8 +1374,14 @@
       <c r="E15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F15" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1302,8 +1397,14 @@
       <c r="E16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1319,8 +1420,14 @@
       <c r="E17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1336,8 +1443,14 @@
       <c r="E18" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1353,11 +1466,17 @@
       <c r="E19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G19" t="s">
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1373,9 +1492,15 @@
       <c r="E20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>0</v>
       </c>
@@ -1398,11 +1523,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="29" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="45">
         <v>4</v>
       </c>
       <c r="C24" s="7">
@@ -1421,9 +1546,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="33"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="43"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="6">
         <v>0.3</v>
       </c>
@@ -1440,9 +1565,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="31"/>
-      <c r="B26" s="34"/>
+    <row r="26" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="44"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="10">
         <v>0.5</v>
       </c>
@@ -1459,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>22</v>
       </c>
@@ -1472,11 +1597,11 @@
       <c r="F27" s="16"/>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="45">
         <v>4</v>
       </c>
       <c r="C28" s="7">
@@ -1495,9 +1620,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="30"/>
-      <c r="B29" s="33"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="43"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="6">
         <v>0.3</v>
       </c>
@@ -1514,9 +1639,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="31"/>
-      <c r="B30" s="34"/>
+    <row r="30" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="44"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="10">
         <v>0.5</v>
       </c>
@@ -1533,11 +1658,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="32">
+      <c r="B31" s="45">
         <v>3</v>
       </c>
       <c r="C31" s="7">
@@ -1556,9 +1681,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
-      <c r="B32" s="33"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="43"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="6">
         <v>0.3</v>
       </c>
@@ -1575,9 +1700,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="31"/>
-      <c r="B33" s="34"/>
+    <row r="33" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="10">
         <v>0.5</v>
       </c>
@@ -1594,11 +1719,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="45">
         <v>3</v>
       </c>
       <c r="C34" s="7">
@@ -1617,9 +1742,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
-      <c r="B35" s="33"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="43"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="6">
         <v>0.3</v>
       </c>
@@ -1636,9 +1761,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="31"/>
-      <c r="B36" s="34"/>
+    <row r="36" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="10">
         <v>0.5</v>
       </c>
@@ -1655,11 +1780,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="29" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="32">
+      <c r="B37" s="45">
         <v>2</v>
       </c>
       <c r="C37" s="7">
@@ -1678,9 +1803,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="30"/>
-      <c r="B38" s="33"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="43"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6">
         <v>0.3</v>
       </c>
@@ -1697,9 +1822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="31"/>
-      <c r="B39" s="34"/>
+    <row r="39" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="44"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="10">
         <v>0.5</v>
       </c>
@@ -1716,11 +1841,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="29" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="32">
+      <c r="B40" s="45">
         <v>2</v>
       </c>
       <c r="C40" s="7">
@@ -1739,9 +1864,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="30"/>
-      <c r="B41" s="33"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="43"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="6">
         <v>0.3</v>
       </c>
@@ -1758,9 +1883,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="31"/>
-      <c r="B42" s="34"/>
+    <row r="42" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="44"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="10">
         <v>0.5</v>
       </c>
@@ -1777,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1915,7 @@
       <c r="F43" s="25"/>
       <c r="G43" s="27"/>
     </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>25</v>
       </c>
@@ -1818,59 +1943,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="40" t="s">
+    <row r="45" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="40" t="s">
+      <c r="C46" s="45"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="41"/>
-      <c r="B47" s="37">
+    <row r="47" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="48"/>
+      <c r="B47" s="30">
         <v>0.1</v>
       </c>
       <c r="C47" s="10">
         <v>0.3</v>
       </c>
-      <c r="D47" s="46">
+      <c r="D47" s="36">
         <v>0.5</v>
       </c>
-      <c r="E47" s="41"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="42" t="s">
+      <c r="E47" s="48"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="31">
         <f>SUM(D28,D31,D34,D37,D40)/(SUM(D28,D31,D34,D37,D40)+SUM(G40,G37,G34,G31,G28,G24))</f>
         <v>0.69230769230769229</v>
       </c>
-      <c r="C48" s="35">
+      <c r="C48" s="29">
         <f>SUM(D29,D32,D35,D38,D41)/(SUM(D29,D32,D35,D38,D41)+SUM(G25,G29,G32,G35,G38,G41))</f>
         <v>0.69230769230769229</v>
       </c>
-      <c r="D48" s="47">
+      <c r="D48" s="37">
         <f>SUM(D30,D33,D36,D39,D42)/(SUM(D30,D33,D36,D39,D42)+SUM(G26,G30,G33,G36,G39,G42))</f>
         <v>0.77777777777777779</v>
       </c>
-      <c r="E48" s="42">
+      <c r="E48" s="33">
         <f>D44/(D44+G44)</f>
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="39">
+      <c r="B49" s="32">
         <f>SUM(D28,D31,D34,D37,D40)/(SUM(D28,D31,D34,D37,D40)+SUM(E40,E37,E34,E31,E28,E24))</f>
         <v>0.81818181818181823</v>
       </c>
@@ -1878,20 +2003,20 @@
         <f>SUM(D29,D32,D35,D38,D41)/(SUM(D29,D32,D35,D38,D41)+SUM(E25,E29,E32,E35,E38,E41))</f>
         <v>0.81818181818181823</v>
       </c>
-      <c r="D49" s="48">
+      <c r="D49" s="38">
         <f>SUM(D30,D33,D36,D39,D42)/(SUM(D30,D33,D36,D39,D42)+SUM(E26,E30,E33,E36,E39,E42))</f>
         <v>0.53846153846153844</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="34">
         <f>D44/(D44+E44)</f>
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="43" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="39">
+      <c r="B50" s="32">
         <f>(SUM(D28,D31,D34,D37,D40)+F24)/SUM(B24,B28,B31,B34,B37,B40)</f>
         <v>0.66666666666666663</v>
       </c>
@@ -1899,20 +2024,20 @@
         <f>(SUM(D29,D32,D35,D38,D41)+F25)/SUM(B24,B28,B31,B34,B37,B40)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D50" s="48">
+      <c r="D50" s="38">
         <f>(SUM(D30,D33,D36,D39,D42)+F26)/SUM(B24,B28,B31,B34,B37,B40)</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="34">
         <f>(D44+F44)/B44</f>
         <v>0.62962962962962965</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="43" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="39">
+      <c r="B51" s="32">
         <f>F24/(F24+SUM(E24,E28,E31,E34,E37,E40))</f>
         <v>0.6</v>
       </c>
@@ -1920,40 +2045,40 @@
         <f>F25/(F25+SUM(E25,E29,E32,E35,E38,E41))</f>
         <v>0.6</v>
       </c>
-      <c r="D51" s="48">
+      <c r="D51" s="38">
         <f>F26/(F26+SUM(E26,E30,E33,E36,E39,E42))</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="34">
         <f>F44/(E44+F44)</f>
         <v>0.47368421052631576</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="44" t="s">
+    <row r="52" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="37">
+      <c r="B52" s="30">
         <f>2*(B48*B49)/(B48+B49)</f>
         <v>0.75000000000000011</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="30">
         <f>2*(C48*C49)/(C48+C49)</f>
         <v>0.75000000000000011</v>
       </c>
-      <c r="D52" s="37">
+      <c r="D52" s="30">
         <f>2*(D48*D49)/(D48+D49)</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="E52" s="44">
+      <c r="E52" s="35">
         <f>2*(E48*E49)/(E48+E49)</f>
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="49"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="39"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F56" t="s">
         <v>35</v>
       </c>
@@ -1965,11 +2090,6 @@
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="A31:A33"/>
@@ -1978,6 +2098,11 @@
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>